<commit_message>
fix mis-uploaded cpu microcontroller code
</commit_message>
<xml_diff>
--- a/Exp04_CPU/微指令自动生成.xlsx
+++ b/Exp04_CPU/微指令自动生成.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="611"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="611"/>
   </bookViews>
   <sheets>
     <sheet name="控制存储器数据自动生成" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="96">
   <si>
     <t>IorD</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -358,6 +358,26 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[rs] OP R[rt], if ture, C → PC (get EQ) (AluSrcA='R[rs]', AluSrcB='R[rt]', BEQ)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C → R[rd] (RegWrite, MemToReg='ALU', RegDst='R[rd]')</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -370,27 +390,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>R[rs] OP R[rt], if ture, C → PC (get EQ) (AluSrcA='R[rs]', AluSrcB='R[rt]', BEQ)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C → R[rd] (RegWrite, MemToReg='ALU', RegDst='R[rd]')</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0</t>
+    <t>11</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -732,6 +736,7 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -741,7 +746,6 @@
     <xf numFmtId="49" fontId="5" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1182,39 +1186,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.875" customWidth="1"/>
-    <col min="2" max="2" width="4.875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.75" style="4" customWidth="1"/>
-    <col min="4" max="4" width="5.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.125" style="1" customWidth="1"/>
-    <col min="9" max="10" width="5.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5.75" style="1" customWidth="1"/>
-    <col min="12" max="12" width="7.25" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="2" max="2" width="4.88671875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="5.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="1" customWidth="1"/>
+    <col min="9" max="10" width="5.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="5.77734375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="7.21875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" style="1" customWidth="1"/>
     <col min="14" max="14" width="8" style="1" customWidth="1"/>
-    <col min="15" max="15" width="5.25" style="1" customWidth="1"/>
+    <col min="15" max="15" width="5.21875" style="1" customWidth="1"/>
     <col min="16" max="16" width="5" style="1" customWidth="1"/>
-    <col min="17" max="17" width="7.375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="3.375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5" style="1" customWidth="1"/>
-    <col min="20" max="20" width="22.25" style="4" customWidth="1"/>
-    <col min="21" max="21" width="8.75" style="5" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="9.625" customWidth="1"/>
-    <col min="23" max="23" width="1.375" customWidth="1"/>
-    <col min="24" max="24" width="8.875" customWidth="1"/>
+    <col min="17" max="17" width="7.33203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="3.33203125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="10.44140625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="22.21875" style="4" customWidth="1"/>
+    <col min="21" max="21" width="8.77734375" style="5" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="9.6640625" customWidth="1"/>
+    <col min="23" max="23" width="1.33203125" customWidth="1"/>
+    <col min="24" max="24" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:24" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>42</v>
       </c>
@@ -1282,7 +1286,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -1353,11 +1357,11 @@
         <f>DEC2HEX(U3)</f>
         <v>13201</v>
       </c>
-      <c r="X3" s="30" t="s">
+      <c r="X3" s="27" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>12</v>
       </c>
@@ -1378,7 +1382,7 @@
         <v>76</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="H4" s="19" t="s">
         <v>34</v>
@@ -1418,21 +1422,21 @@
       </c>
       <c r="T4" s="11" t="str">
         <f t="shared" ref="T4:T16" si="1">D4&amp;E4&amp;F4&amp;G4&amp;H4&amp;I4&amp;J4&amp;K4&amp;L4&amp;M4&amp;N4&amp;O4&amp;P4&amp;Q4&amp;R4&amp;S4</f>
-        <v>000100000000000010000</v>
+        <v>000110000000000010000</v>
       </c>
       <c r="U4" s="12">
         <f t="shared" ref="U4:U16" si="2">BIN2DEC(LEFT(T4,LEN(T4)-16))*256*256+BIN2DEC(MID(T4,LEN(T4)-15,8))*256+BIN2DEC(MID(T4,LEN(T4)-7,8))</f>
-        <v>131088</v>
+        <v>196624</v>
       </c>
       <c r="V4" s="10" t="str">
         <f t="shared" ref="V4:V16" si="3">DEC2HEX(U4)</f>
-        <v>20010</v>
-      </c>
-      <c r="X4" s="30" t="s">
+        <v>30010</v>
+      </c>
+      <c r="X4" s="27" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -1503,11 +1507,11 @@
         <f>DEC2HEX(U5)</f>
         <v>60003</v>
       </c>
-      <c r="X5" s="30" t="s">
+      <c r="X5" s="27" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>25</v>
       </c>
@@ -1578,11 +1582,11 @@
         <f t="shared" si="3"/>
         <v>130204</v>
       </c>
-      <c r="X6" s="30" t="s">
+      <c r="X6" s="27" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -1653,11 +1657,11 @@
         <f t="shared" si="3"/>
         <v>38800</v>
       </c>
-      <c r="X7" s="30" t="s">
+      <c r="X7" s="27" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>27</v>
       </c>
@@ -1728,11 +1732,11 @@
         <f t="shared" si="3"/>
         <v>60006</v>
       </c>
-      <c r="X8" s="30" t="s">
+      <c r="X8" s="27" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -1803,11 +1807,11 @@
         <f t="shared" si="3"/>
         <v>130400</v>
       </c>
-      <c r="X9" s="30" t="s">
+      <c r="X9" s="27" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>43</v>
       </c>
@@ -1878,11 +1882,11 @@
         <f t="shared" si="3"/>
         <v>40048</v>
       </c>
-      <c r="X10" s="30" t="s">
+      <c r="X10" s="27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>44</v>
       </c>
@@ -1906,7 +1910,7 @@
         <v>39</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="I11" s="19" t="s">
         <v>66</v>
@@ -1943,21 +1947,21 @@
       </c>
       <c r="T11" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>000111100100000000000</v>
+        <v>000110100100000000000</v>
       </c>
       <c r="U11" s="7">
         <f t="shared" si="2"/>
-        <v>247808</v>
+        <v>215040</v>
       </c>
       <c r="V11" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>3C800</v>
-      </c>
-      <c r="X11" s="30" t="s">
+        <v>34800</v>
+      </c>
+      <c r="X11" s="27" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>29</v>
       </c>
@@ -1969,7 +1973,7 @@
         <v>1001</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>58</v>
@@ -2028,11 +2032,11 @@
         <f t="shared" si="3"/>
         <v>C0100</v>
       </c>
-      <c r="X12" s="30" t="s">
-        <v>89</v>
+      <c r="X12" s="27" t="s">
+        <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
@@ -2044,7 +2048,7 @@
         <v>1010</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>61</v>
@@ -2103,9 +2107,9 @@
         <f t="shared" si="3"/>
         <v>C0080</v>
       </c>
-      <c r="X13" s="30"/>
+      <c r="X13" s="27"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>31</v>
       </c>
@@ -2126,7 +2130,7 @@
         <v>47</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H14" s="19" t="s">
         <v>34</v>
@@ -2176,11 +2180,11 @@
         <f t="shared" si="3"/>
         <v>6000C</v>
       </c>
-      <c r="X14" s="30" t="s">
+      <c r="X14" s="27" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
@@ -2204,10 +2208,10 @@
         <v>39</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J15" s="19" t="s">
         <v>34</v>
@@ -2216,7 +2220,7 @@
         <v>34</v>
       </c>
       <c r="L15" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M15" s="19" t="s">
         <v>34</v>
@@ -2251,11 +2255,11 @@
         <f t="shared" si="3"/>
         <v>30800</v>
       </c>
-      <c r="X15" s="30" t="s">
-        <v>91</v>
+      <c r="X15" s="27" t="s">
+        <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>33</v>
       </c>
@@ -2326,46 +2330,46 @@
         <f t="shared" si="3"/>
         <v>D</v>
       </c>
-      <c r="X16" s="30"/>
+      <c r="X16" s="27"/>
     </row>
-    <row r="17" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:20" x14ac:dyDescent="0.25">
       <c r="T17" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:20" x14ac:dyDescent="0.25">
       <c r="T18" s="14">
         <f>LEN(T16)</f>
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:20" x14ac:dyDescent="0.25">
       <c r="Q20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="4:20" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="4:20" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="27" t="s">
+    <row r="21" spans="4:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="4:20" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="28"/>
-      <c r="S22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="29"/>
+      <c r="R22" s="29"/>
+      <c r="S22" s="30"/>
     </row>
-    <row r="23" spans="4:20" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="4:20" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <protectedRanges>
     <protectedRange sqref="D1:S1048576" name="区域1"/>

</xml_diff>